<commit_message>
add final tweaks to MLM results for screenshots
</commit_message>
<xml_diff>
--- a/machine_learning/results_main.xlsx
+++ b/machine_learning/results_main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lbjork/Desktop/Traffic_Analysis/machine_learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDD64E72-D169-8B40-842D-F32A3659F44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C04ADA-EE12-7D49-98C5-D4A830BFE692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33020" yWindow="2560" windowWidth="28040" windowHeight="17040" activeTab="2" xr2:uid="{02AE315F-9872-B444-86A2-12D1EAD157CC}"/>
+    <workbookView xWindow="33020" yWindow="2560" windowWidth="28040" windowHeight="17040" activeTab="5" xr2:uid="{02AE315F-9872-B444-86A2-12D1EAD157CC}"/>
   </bookViews>
   <sheets>
     <sheet name="source_injury_type" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,12 @@
     <sheet name="accuracy_table" sheetId="4" r:id="rId3"/>
     <sheet name="injury_type_scores" sheetId="5" r:id="rId4"/>
     <sheet name="crash_severity_scores" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">source_injury_type!$A$7:$E$17</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="70">
   <si>
     <t>Classification Report</t>
   </si>
@@ -172,6 +173,84 @@
   </si>
   <si>
     <t>Rounded Accuracy Score</t>
+  </si>
+  <si>
+    <t>Statewide Data</t>
+  </si>
+  <si>
+    <t>Clark County Data</t>
+  </si>
+  <si>
+    <t>All Columns</t>
+  </si>
+  <si>
+    <t>Top 50%</t>
+  </si>
+  <si>
+    <t>Clark County</t>
+  </si>
+  <si>
+    <t>Accuracy Scores</t>
+  </si>
+  <si>
+    <t>Top 16</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>v1_driver_age</t>
+  </si>
+  <si>
+    <t>v2_driver_age</t>
+  </si>
+  <si>
+    <t>crash_day</t>
+  </si>
+  <si>
+    <t>crash_hour</t>
+  </si>
+  <si>
+    <t>crash_month</t>
+  </si>
+  <si>
+    <t>crash_day_of_week</t>
+  </si>
+  <si>
+    <t>crash_year</t>
+  </si>
+  <si>
+    <t>factors_roadway_1_UNKNOWN</t>
+  </si>
+  <si>
+    <t>factors_roadway_1_DRY</t>
+  </si>
+  <si>
+    <t>lighting_UNKNOWN</t>
+  </si>
+  <si>
+    <t>total_vehicles</t>
+  </si>
+  <si>
+    <t>lighting_DAYLIGHT</t>
+  </si>
+  <si>
+    <t>hwy_factors_1_NONE</t>
+  </si>
+  <si>
+    <t>v1_type_SEDAN_4DOOR</t>
+  </si>
+  <si>
+    <t>hwy_factors_1_UNKNOWN</t>
+  </si>
+  <si>
+    <t>injury_type</t>
+  </si>
+  <si>
+    <t>crash_severity</t>
   </si>
 </sst>
 </file>
@@ -1522,137 +1601,189 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57BF027-A91F-0643-B6AB-5387AE315A93}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E19:E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="4" width="33.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="C2">
+      <c r="B3">
         <v>1345</v>
       </c>
-      <c r="D2">
+      <c r="C3">
         <v>0.74000744456458101</v>
       </c>
-      <c r="E2">
-        <f>ROUND(D2,2)</f>
+      <c r="D3">
+        <f>ROUND(C3,2)</f>
         <v>0.74</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>35</v>
       </c>
-      <c r="C3">
+      <c r="B4">
         <v>773</v>
       </c>
-      <c r="D3">
+      <c r="C4">
         <v>0.73422904443696002</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">ROUND(D3,2)</f>
+      <c r="D4">
+        <f t="shared" ref="D4:D7" si="0">ROUND(C4,2)</f>
         <v>0.73</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
         <v>1345</v>
       </c>
-      <c r="D4">
-        <v>0.74116122953715702</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>1345</v>
-      </c>
-      <c r="D5">
+      <c r="C6">
         <v>0.65668149671198395</v>
       </c>
-      <c r="E5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="C6">
+      <c r="B7">
         <v>773</v>
       </c>
-      <c r="D6">
+      <c r="C7">
         <v>0.65538756048708702</v>
       </c>
-      <c r="E6">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>1232</v>
+      </c>
+      <c r="C12">
+        <v>0.74116122953715702</v>
+      </c>
+      <c r="D12">
+        <f>ROUND(C12,2)</f>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="C7">
-        <v>1345</v>
-      </c>
-      <c r="D7">
+      <c r="B13">
+        <v>1232</v>
+      </c>
+      <c r="C13">
         <v>0.64609586621128201</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="D13">
+        <f>ROUND(C13,2)</f>
         <v>0.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>0.66</v>
+      </c>
+      <c r="C19">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>0.74</v>
+      </c>
+      <c r="C20">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>0.74</v>
       </c>
     </row>
   </sheetData>
@@ -1666,7 +1797,7 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1048576"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1789,8 +1920,8 @@
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="3">
-        <v>1345</v>
+      <c r="D5">
+        <v>1232</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -1981,8 +2112,8 @@
       <c r="C11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="3">
-        <v>1345</v>
+      <c r="D11">
+        <v>1232</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -2014,7 +2145,7 @@
   <dimension ref="A3:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2109,7 +2240,7 @@
         <v>35</v>
       </c>
       <c r="D6">
-        <v>1345</v>
+        <v>1232</v>
       </c>
       <c r="E6">
         <v>0.77</v>
@@ -2247,7 +2378,7 @@
         <v>35</v>
       </c>
       <c r="D12">
-        <v>1345</v>
+        <v>1232</v>
       </c>
       <c r="E12">
         <v>0.76</v>
@@ -2262,4 +2393,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EE2E1C-8650-F449-8306-9B0D1D1DF958}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="2" width="37.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
+    <sortCondition ref="B2:B19"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>